<commit_message>
updated CheckList Table in consideration of requirement.
</commit_message>
<xml_diff>
--- a/GoodAndBetter_Schema.xlsx
+++ b/GoodAndBetter_Schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="Shema" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="137">
   <si>
     <t>version</t>
   </si>
@@ -482,6 +482,18 @@
   </si>
   <si>
     <t>get 방식 : http://wan.iptime.org:5001/appAboutPlant?clientCode=2&amp;plantCode=1</t>
+  </si>
+  <si>
+    <t>CHE_Cleanleaf</t>
+  </si>
+  <si>
+    <t>입세정</t>
+  </si>
+  <si>
+    <t>CHE_Change</t>
+  </si>
+  <si>
+    <t>교체</t>
   </si>
 </sst>
 </file>
@@ -1189,6 +1201,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1273,6 +1288,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1288,14 +1384,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1306,78 +1402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1396,14 +1420,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1432,11 +1453,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1474,15 +1498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1492,12 +1507,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1506,9 +1521,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1839,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="K8" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18:Q18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1866,50 +1878,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="60"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="62"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="58"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="5">
         <v>42181</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="67"/>
       <c r="K5" s="6">
         <v>42175</v>
       </c>
@@ -1951,13 +1963,13 @@
       <c r="I9" s="1"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="72" t="s">
+      <c r="O9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="74"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="70"/>
     </row>
     <row r="10" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1989,11 +2001,11 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="77"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="73"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2025,11 +2037,11 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="48"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="76"/>
       <c r="R11" s="7" t="s">
         <v>10</v>
       </c>
@@ -2055,11 +2067,11 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="49" t="s">
+      <c r="O12" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="50"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="78"/>
       <c r="R12" s="14" t="s">
         <v>83</v>
       </c>
@@ -2093,11 +2105,11 @@
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="51" t="s">
+      <c r="O13" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="53"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="49"/>
       <c r="R13" s="14" t="s">
         <v>85</v>
       </c>
@@ -2108,11 +2120,11 @@
     <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
-      <c r="O14" s="51" t="s">
+      <c r="O14" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="53"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="14" t="s">
         <v>106</v>
       </c>
@@ -2137,15 +2149,15 @@
       <c r="J15" s="1"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
-      <c r="O15" s="89" t="s">
+      <c r="O15" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="87" t="s">
+      <c r="P15" s="48"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="S15" s="88">
+      <c r="S15" s="51">
         <v>42192</v>
       </c>
     </row>
@@ -2166,11 +2178,11 @@
       <c r="J16" s="1"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="87"/>
-      <c r="S16" s="88"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="51"/>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2205,13 +2217,13 @@
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
-      <c r="O17" s="54" t="s">
+      <c r="O17" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="87"/>
-      <c r="S17" s="88"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="51"/>
     </row>
     <row r="18" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2246,9 +2258,9 @@
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="80"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="81"/>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
@@ -2271,9 +2283,9 @@
       <c r="J19" s="1"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="80"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="81"/>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
@@ -2308,36 +2320,36 @@
       </c>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="83"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="86"/>
+      <c r="Q20" s="87"/>
       <c r="R20" s="14"/>
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="56"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="84"/>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="56"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="84"/>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="56"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="84"/>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
@@ -2355,11 +2367,12 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="M24" s="12"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="56"/>
+      <c r="O24" s="82"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="84"/>
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
@@ -2377,11 +2390,12 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="M25" s="12"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="56"/>
+      <c r="O25" s="82"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="84"/>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
@@ -2405,19 +2419,24 @@
         <v>60</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M26" s="11"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="54"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="56"/>
+      <c r="O26" s="82"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="84"/>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
@@ -2444,16 +2463,21 @@
         <v>92</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M27" s="11"/>
       <c r="N27" s="11"/>
-      <c r="O27" s="81"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="83"/>
+      <c r="O27" s="85"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="87"/>
       <c r="R27" s="14"/>
       <c r="S27" s="5"/>
     </row>
@@ -2470,14 +2494,15 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M28" s="11"/>
       <c r="N28" s="11"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="83"/>
+      <c r="O28" s="85"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="87"/>
       <c r="R28" s="14"/>
       <c r="S28" s="5"/>
     </row>
@@ -2501,44 +2526,49 @@
         <v>90</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="M29" s="11"/>
+      <c r="K29" s="1"/>
       <c r="N29" s="11"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="83"/>
+      <c r="O29" s="85"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="87"/>
       <c r="R29" s="14"/>
       <c r="S29" s="4"/>
     </row>
     <row r="30" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="83"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="86"/>
+      <c r="Q30" s="87"/>
       <c r="R30" s="14"/>
       <c r="S30" s="4"/>
     </row>
     <row r="31" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
-      <c r="O31" s="81"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="83"/>
+      <c r="O31" s="85"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="87"/>
       <c r="R31" s="14"/>
       <c r="S31" s="4"/>
     </row>
     <row r="32" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
-      <c r="O32" s="81"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="83"/>
+      <c r="O32" s="85"/>
+      <c r="P32" s="86"/>
+      <c r="Q32" s="87"/>
       <c r="R32" s="14"/>
       <c r="S32" s="4"/>
     </row>
@@ -2563,9 +2593,9 @@
       <c r="K33" s="1"/>
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="83"/>
+      <c r="O33" s="85"/>
+      <c r="P33" s="86"/>
+      <c r="Q33" s="87"/>
       <c r="R33" s="14"/>
       <c r="S33" s="4"/>
     </row>
@@ -2590,9 +2620,9 @@
       <c r="K34" s="1"/>
       <c r="M34" s="11"/>
       <c r="N34" s="11"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="82"/>
-      <c r="Q34" s="83"/>
+      <c r="O34" s="85"/>
+      <c r="P34" s="86"/>
+      <c r="Q34" s="87"/>
       <c r="R34" s="14"/>
       <c r="S34" s="4"/>
     </row>
@@ -2629,9 +2659,9 @@
       </c>
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="82"/>
-      <c r="Q35" s="83"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="87"/>
       <c r="R35" s="14"/>
       <c r="S35" s="4"/>
     </row>
@@ -2666,9 +2696,9 @@
       </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
-      <c r="O36" s="81"/>
-      <c r="P36" s="82"/>
-      <c r="Q36" s="83"/>
+      <c r="O36" s="85"/>
+      <c r="P36" s="86"/>
+      <c r="Q36" s="87"/>
       <c r="R36" s="14"/>
       <c r="S36" s="4"/>
     </row>
@@ -2697,9 +2727,9 @@
       <c r="K37" s="1"/>
       <c r="M37" s="11"/>
       <c r="N37" s="11"/>
-      <c r="O37" s="81"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="83"/>
+      <c r="O37" s="85"/>
+      <c r="P37" s="86"/>
+      <c r="Q37" s="87"/>
       <c r="R37" s="14"/>
       <c r="S37" s="4"/>
     </row>
@@ -2726,9 +2756,9 @@
       <c r="K38" s="1"/>
       <c r="M38" s="11"/>
       <c r="N38" s="11"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="83"/>
+      <c r="O38" s="85"/>
+      <c r="P38" s="86"/>
+      <c r="Q38" s="87"/>
       <c r="R38" s="14"/>
       <c r="S38" s="4"/>
     </row>
@@ -2737,9 +2767,9 @@
       <c r="J39" s="9"/>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
-      <c r="O39" s="81"/>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="83"/>
+      <c r="O39" s="85"/>
+      <c r="P39" s="86"/>
+      <c r="Q39" s="87"/>
       <c r="R39" s="14"/>
       <c r="S39" s="4"/>
     </row>
@@ -2748,154 +2778,154 @@
       <c r="J40" s="9"/>
       <c r="M40" s="11"/>
       <c r="N40" s="11"/>
-      <c r="O40" s="81"/>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="83"/>
+      <c r="O40" s="85"/>
+      <c r="P40" s="86"/>
+      <c r="Q40" s="87"/>
       <c r="R40" s="14"/>
       <c r="S40" s="4"/>
     </row>
     <row r="41" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="O41" s="84"/>
-      <c r="P41" s="85"/>
-      <c r="Q41" s="86"/>
+      <c r="O41" s="88"/>
+      <c r="P41" s="89"/>
+      <c r="Q41" s="90"/>
       <c r="R41" s="16"/>
       <c r="S41" s="17"/>
     </row>
     <row r="43" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="33"/>
     </row>
     <row r="45" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="33"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="35"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="36"/>
     </row>
     <row r="46" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="40"/>
     </row>
     <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="37"/>
-      <c r="C47" s="40" t="s">
+      <c r="B47" s="38"/>
+      <c r="C47" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="43"/>
     </row>
     <row r="48" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="37"/>
-      <c r="C48" s="43" t="s">
+      <c r="B48" s="38"/>
+      <c r="C48" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="46"/>
     </row>
     <row r="49" spans="2:12" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="24"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B50" s="19"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="25"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="26"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B51" s="19"/>
-      <c r="C51" s="26" t="s">
+      <c r="B51" s="20"/>
+      <c r="C51" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="28"/>
     </row>
     <row r="52" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
-      <c r="C52" s="28" t="s">
+      <c r="B52" s="21"/>
+      <c r="C52" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="46">
@@ -2955,30 +2985,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:S35"/>
+  <dimension ref="B3:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33:R33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-    </row>
-    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-    </row>
-    <row r="5" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="2:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="120" t="s">
         <v>126</v>
       </c>
@@ -2988,531 +3018,531 @@
       <c r="F5" s="120"/>
       <c r="G5" s="120"/>
       <c r="H5" s="120"/>
-      <c r="L5" s="124" t="s">
+      <c r="L5" s="121" t="s">
         <v>132</v>
       </c>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="90" t="s">
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="93" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="92"/>
-      <c r="L7" s="90" t="s">
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
+      <c r="L7" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="93"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="95"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="94"/>
-      <c r="R8" s="95"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="96" t="s">
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="95"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="98"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="97"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="98"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="99" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="98"/>
-      <c r="L9" s="96" t="s">
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
+      <c r="L9" s="99" t="s">
         <v>119</v>
       </c>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="98"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="99" t="s">
+      <c r="M9" s="100"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="100"/>
+      <c r="R9" s="101"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
-      <c r="L10" s="99" t="s">
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87"/>
+      <c r="L10" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="83"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="99" t="s">
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="87"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
-      <c r="L11" s="99" t="s">
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="L11" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="M11" s="82"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
-      <c r="P11" s="82"/>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="83"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="99" t="s">
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="87"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
-      <c r="L12" s="99" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="L12" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="83"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="100" t="s">
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="87"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="53"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="99" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="49"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="L14" s="99" t="s">
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="87"/>
+      <c r="L14" s="91" t="s">
         <v>128</v>
       </c>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="82"/>
-      <c r="R14" s="83"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="99" t="s">
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="87"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="83"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="83"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="101" t="s">
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="87"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="87"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="103"/>
-      <c r="L16" s="101" t="s">
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="107"/>
+      <c r="L16" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="103"/>
+      <c r="M16" s="106"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="106"/>
+      <c r="P16" s="106"/>
+      <c r="Q16" s="106"/>
+      <c r="R16" s="107"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="106"/>
-      <c r="L17" s="104" t="s">
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="110"/>
+      <c r="L17" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="M17" s="105"/>
-      <c r="N17" s="105"/>
-      <c r="O17" s="105"/>
-      <c r="P17" s="105"/>
-      <c r="Q17" s="105"/>
-      <c r="R17" s="106"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="109"/>
+      <c r="O17" s="109"/>
+      <c r="P17" s="109"/>
+      <c r="Q17" s="109"/>
+      <c r="R17" s="110"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="107"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="109"/>
-      <c r="L18" s="107"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="108"/>
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="109"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="113"/>
+      <c r="L18" s="111"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="113"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="114" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="112"/>
-      <c r="L19" s="110" t="s">
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="116"/>
+      <c r="L19" s="114" t="s">
         <v>122</v>
       </c>
-      <c r="M19" s="111"/>
-      <c r="N19" s="111"/>
-      <c r="O19" s="111"/>
-      <c r="P19" s="111"/>
-      <c r="Q19" s="111"/>
-      <c r="R19" s="112"/>
+      <c r="M19" s="115"/>
+      <c r="N19" s="115"/>
+      <c r="O19" s="115"/>
+      <c r="P19" s="115"/>
+      <c r="Q19" s="115"/>
+      <c r="R19" s="116"/>
     </row>
     <row r="20" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="113" t="s">
+      <c r="B20" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="115"/>
-      <c r="L20" s="121" t="s">
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
+      <c r="L20" s="122" t="s">
         <v>131</v>
       </c>
-      <c r="M20" s="122"/>
-      <c r="N20" s="122"/>
-      <c r="O20" s="122"/>
-      <c r="P20" s="122"/>
-      <c r="Q20" s="122"/>
-      <c r="R20" s="123"/>
+      <c r="M20" s="123"/>
+      <c r="N20" s="123"/>
+      <c r="O20" s="123"/>
+      <c r="P20" s="123"/>
+      <c r="Q20" s="123"/>
+      <c r="R20" s="124"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="113"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="114"/>
-      <c r="H21" s="115"/>
-      <c r="L21" s="121"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="122"/>
-      <c r="O21" s="122"/>
-      <c r="P21" s="122"/>
-      <c r="Q21" s="122"/>
-      <c r="R21" s="123"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="104"/>
+      <c r="L21" s="122"/>
+      <c r="M21" s="123"/>
+      <c r="N21" s="123"/>
+      <c r="O21" s="123"/>
+      <c r="P21" s="123"/>
+      <c r="Q21" s="123"/>
+      <c r="R21" s="124"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="113" t="s">
+      <c r="B22" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="114"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="115"/>
-      <c r="L22" s="121"/>
-      <c r="M22" s="122"/>
-      <c r="N22" s="122"/>
-      <c r="O22" s="122"/>
-      <c r="P22" s="122"/>
-      <c r="Q22" s="122"/>
-      <c r="R22" s="123"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="104"/>
+      <c r="L22" s="122"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="123"/>
+      <c r="O22" s="123"/>
+      <c r="P22" s="123"/>
+      <c r="Q22" s="123"/>
+      <c r="R22" s="124"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="113" t="s">
+      <c r="B23" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="114"/>
-      <c r="H23" s="115"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="122"/>
-      <c r="N23" s="122"/>
-      <c r="O23" s="122"/>
-      <c r="P23" s="122"/>
-      <c r="Q23" s="122"/>
-      <c r="R23" s="123"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="104"/>
+      <c r="L23" s="122"/>
+      <c r="M23" s="123"/>
+      <c r="N23" s="123"/>
+      <c r="O23" s="123"/>
+      <c r="P23" s="123"/>
+      <c r="Q23" s="123"/>
+      <c r="R23" s="124"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="113"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="115"/>
-      <c r="L24" s="121"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="123"/>
+      <c r="B24" s="102"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="104"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="123"/>
+      <c r="P24" s="123"/>
+      <c r="Q24" s="123"/>
+      <c r="R24" s="124"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="113"/>
-      <c r="C25" s="114"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
-      <c r="G25" s="114"/>
-      <c r="H25" s="115"/>
-      <c r="L25" s="121"/>
-      <c r="M25" s="122"/>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122"/>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="122"/>
-      <c r="R25" s="123"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="104"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="123"/>
+      <c r="N25" s="123"/>
+      <c r="O25" s="123"/>
+      <c r="P25" s="123"/>
+      <c r="Q25" s="123"/>
+      <c r="R25" s="124"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="113"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="114"/>
-      <c r="H26" s="115"/>
-      <c r="L26" s="121"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-      <c r="P26" s="122"/>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="123"/>
+      <c r="B26" s="102"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="104"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="123"/>
+      <c r="N26" s="123"/>
+      <c r="O26" s="123"/>
+      <c r="P26" s="123"/>
+      <c r="Q26" s="123"/>
+      <c r="R26" s="124"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="113"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="115"/>
-      <c r="L27" s="121"/>
-      <c r="M27" s="122"/>
-      <c r="N27" s="122"/>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="123"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="123"/>
+      <c r="N27" s="123"/>
+      <c r="O27" s="123"/>
+      <c r="P27" s="123"/>
+      <c r="Q27" s="123"/>
+      <c r="R27" s="124"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="113"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="114"/>
-      <c r="G28" s="114"/>
-      <c r="H28" s="115"/>
-      <c r="L28" s="121"/>
-      <c r="M28" s="122"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="123"/>
+      <c r="B28" s="102"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="123"/>
+      <c r="N28" s="123"/>
+      <c r="O28" s="123"/>
+      <c r="P28" s="123"/>
+      <c r="Q28" s="123"/>
+      <c r="R28" s="124"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="113"/>
-      <c r="C29" s="114"/>
-      <c r="D29" s="114"/>
-      <c r="E29" s="114"/>
-      <c r="F29" s="114"/>
-      <c r="G29" s="114"/>
-      <c r="H29" s="115"/>
-      <c r="L29" s="113"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="114"/>
-      <c r="O29" s="114"/>
-      <c r="P29" s="114"/>
-      <c r="Q29" s="114"/>
-      <c r="R29" s="115"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="103"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="104"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B30" s="113"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="115"/>
-      <c r="L30" s="113"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="114"/>
-      <c r="R30" s="115"/>
+      <c r="B30" s="102"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="104"/>
+      <c r="L30" s="102"/>
+      <c r="M30" s="103"/>
+      <c r="N30" s="103"/>
+      <c r="O30" s="103"/>
+      <c r="P30" s="103"/>
+      <c r="Q30" s="103"/>
+      <c r="R30" s="104"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="113"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="115"/>
-      <c r="L31" s="113" t="s">
+      <c r="B31" s="102"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="104"/>
+      <c r="L31" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="M31" s="114"/>
-      <c r="N31" s="114"/>
-      <c r="O31" s="114"/>
-      <c r="P31" s="114"/>
-      <c r="Q31" s="114"/>
-      <c r="R31" s="115"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="104"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="113"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="115"/>
-      <c r="L32" s="113" t="s">
+      <c r="B32" s="102"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="104"/>
+      <c r="L32" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="M32" s="114"/>
-      <c r="N32" s="114"/>
-      <c r="O32" s="114"/>
-      <c r="P32" s="114"/>
-      <c r="Q32" s="114"/>
-      <c r="R32" s="115"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103"/>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="104"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="113"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="114"/>
-      <c r="G33" s="114"/>
-      <c r="H33" s="115"/>
-      <c r="L33" s="113"/>
-      <c r="M33" s="114"/>
-      <c r="N33" s="114"/>
-      <c r="O33" s="114"/>
-      <c r="P33" s="114"/>
-      <c r="Q33" s="114"/>
-      <c r="R33" s="115"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="104"/>
+      <c r="L33" s="102"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
+      <c r="O33" s="103"/>
+      <c r="P33" s="103"/>
+      <c r="Q33" s="103"/>
+      <c r="R33" s="104"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="113"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="115"/>
-      <c r="L34" s="113"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="114"/>
-      <c r="O34" s="114"/>
-      <c r="P34" s="114"/>
-      <c r="Q34" s="114"/>
-      <c r="R34" s="115"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="104"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="103"/>
+      <c r="P34" s="103"/>
+      <c r="Q34" s="103"/>
+      <c r="R34" s="104"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="116"/>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="118"/>
-      <c r="L35" s="116"/>
-      <c r="M35" s="117"/>
-      <c r="N35" s="117"/>
-      <c r="O35" s="117"/>
-      <c r="P35" s="117"/>
-      <c r="Q35" s="117"/>
-      <c r="R35" s="118"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="119"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="118"/>
+      <c r="N35" s="118"/>
+      <c r="O35" s="118"/>
+      <c r="P35" s="118"/>
+      <c r="Q35" s="118"/>
+      <c r="R35" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="48">
@@ -3531,12 +3561,13 @@
     <mergeCell ref="L16:R16"/>
     <mergeCell ref="L17:R18"/>
     <mergeCell ref="L19:R19"/>
+    <mergeCell ref="L12:R12"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="L7:R8"/>
     <mergeCell ref="L9:R9"/>
     <mergeCell ref="L10:R10"/>
     <mergeCell ref="L11:R11"/>
-    <mergeCell ref="L12:R12"/>
+    <mergeCell ref="B11:H11"/>
     <mergeCell ref="B34:H34"/>
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="B28:H28"/>
@@ -3545,18 +3576,17 @@
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B27:H27"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B17:H18"/>
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="B14:H14"/>

</xml_diff>

<commit_message>
Database Table Major change
Combine Question And Reply Table to TALK table
</commit_message>
<xml_diff>
--- a/GoodAndBetter_Schema.xlsx
+++ b/GoodAndBetter_Schema.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26018"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Wan/Desktop/GoodAndBetter/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Good And Better\git\Good-Better\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565"/>
   </bookViews>
   <sheets>
     <sheet name="Shema" sheetId="3" r:id="rId1"/>
@@ -17,18 +17,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="135">
   <si>
     <t>version</t>
   </si>
@@ -142,9 +142,6 @@
     <t>체크리스트</t>
   </si>
   <si>
-    <t>문의하기</t>
-  </si>
-  <si>
     <t>초기 문서 정리</t>
   </si>
   <si>
@@ -235,63 +232,26 @@
     <t>CHE_Repotting</t>
   </si>
   <si>
+    <t>가능한한 줄임말을 쓰지 않는다. (ex: FAVT (x) -&gt; FAVORITE (o) )            - 단, ID나 NFC 등 약어가 이미 대표말로 쓰일 경우나 테이블 명이 너무 길어질 때는 제외한다.</t>
+  </si>
+  <si>
+    <t>CHE_Indate</t>
+  </si>
+  <si>
+    <t>년월일까지</t>
+  </si>
+  <si>
+    <t>MEM_Isadmin</t>
+  </si>
+  <si>
+    <t>관리자 여부</t>
+  </si>
+  <si>
+    <t>MEM_Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PK</t>
-  </si>
-  <si>
-    <t>QUESTION</t>
-  </si>
-  <si>
-    <t>QUE_Code</t>
-  </si>
-  <si>
-    <t>QUE_Content</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>답변</t>
-  </si>
-  <si>
-    <t>REPLY</t>
-  </si>
-  <si>
-    <t>REP_Code</t>
-  </si>
-  <si>
-    <t>REP_Content</t>
-  </si>
-  <si>
-    <t>REP_InDate</t>
-  </si>
-  <si>
-    <t>가능한한 줄임말을 쓰지 않는다. (ex: FAVT (x) -&gt; FAVORITE (o) )            - 단, ID나 NFC 등 약어가 이미 대표말로 쓰일 경우나 테이블 명이 너무 길어질 때는 제외한다.</t>
-  </si>
-  <si>
-    <t>CHE_Indate</t>
-  </si>
-  <si>
-    <t>년월일까지</t>
-  </si>
-  <si>
-    <t>QUE_Indate</t>
-  </si>
-  <si>
-    <t>MEM_Isadmin</t>
-  </si>
-  <si>
-    <t>관리자 여부</t>
-  </si>
-  <si>
-    <t>MEM_Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -386,10 +346,6 @@
   </si>
   <si>
     <t>굿앤배러 직원.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v 0.1.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -494,6 +450,54 @@
   </si>
   <si>
     <t>교체</t>
+  </si>
+  <si>
+    <t>Q&amp;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TALK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAL_Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAL_Question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLA_Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAL_Questionindate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAL_Reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(1000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAL_Replyindate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v 0.3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질의응답 테이블 1개로 통합.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -504,14 +508,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -534,7 +538,7 @@
       <b/>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -542,7 +546,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -551,7 +555,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -560,7 +564,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -569,7 +573,7 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -577,7 +581,7 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -585,7 +589,7 @@
     <font>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1524,11 +1528,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="3" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1851,33 +1855,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G1" s="53" t="s">
         <v>28</v>
       </c>
@@ -1886,14 +1890,14 @@
       <c r="J1" s="54"/>
       <c r="K1" s="55"/>
     </row>
-    <row r="2" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G2" s="56"/>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
       <c r="J2" s="57"/>
       <c r="K2" s="58"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G3" s="59" t="s">
         <v>0</v>
       </c>
@@ -1901,10 +1905,10 @@
       <c r="I3" s="60"/>
       <c r="J3" s="61"/>
       <c r="K3" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G4" s="62" t="s">
         <v>1</v>
       </c>
@@ -1912,10 +1916,10 @@
       <c r="I4" s="63"/>
       <c r="J4" s="64"/>
       <c r="K4" s="5">
-        <v>42181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G5" s="65" t="s">
         <v>2</v>
       </c>
@@ -1926,8 +1930,8 @@
         <v>42175</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1947,7 +1951,7 @@
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1971,33 +1975,33 @@
       <c r="R9" s="69"/>
       <c r="S9" s="70"/>
     </row>
-    <row r="10" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -2007,7 +2011,7 @@
       <c r="R10" s="72"/>
       <c r="S10" s="73"/>
     </row>
-    <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2018,22 +2022,22 @@
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
@@ -2049,7 +2053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2063,76 +2067,76 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P12" s="45"/>
       <c r="Q12" s="78"/>
       <c r="R12" s="14" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="S12" s="5">
         <v>42175</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="50" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="P13" s="48"/>
       <c r="Q13" s="49"/>
       <c r="R13" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="S13" s="15">
         <v>42177</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="50" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="P14" s="48"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="14" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="S14" s="5">
         <v>42181</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2150,23 +2154,23 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="47" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="P15" s="48"/>
       <c r="Q15" s="49"/>
       <c r="R15" s="52" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="S15" s="51">
         <v>42192</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2184,48 +2188,48 @@
       <c r="R16" s="52"/>
       <c r="S16" s="51"/>
     </row>
-    <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="82" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="P17" s="83"/>
       <c r="Q17" s="84"/>
       <c r="R17" s="52"/>
       <c r="S17" s="51"/>
     </row>
-    <row r="18" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2236,35 +2240,41 @@
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
-      <c r="O18" s="79"/>
+      <c r="O18" s="79" t="s">
+        <v>134</v>
+      </c>
       <c r="P18" s="80"/>
       <c r="Q18" s="81"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="15"/>
-    </row>
-    <row r="19" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R18" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="S18" s="15">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2272,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2289,34 +2299,34 @@
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
-    <row r="20" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
@@ -2326,7 +2336,7 @@
       <c r="R20" s="14"/>
       <c r="S20" s="5"/>
     </row>
-    <row r="21" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="82"/>
@@ -2335,7 +2345,7 @@
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
-    <row r="22" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
       <c r="O22" s="82"/>
@@ -2344,7 +2354,7 @@
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
-    <row r="23" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
       <c r="O23" s="82"/>
@@ -2353,7 +2363,7 @@
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
-    <row r="24" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2376,12 +2386,12 @@
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
-    <row r="25" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2399,39 +2409,39 @@
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
-    <row r="26" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N26" s="11"/>
       <c r="O26" s="82"/>
@@ -2440,7 +2450,7 @@
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
-    <row r="27" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2448,28 +2458,28 @@
         <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>18</v>
@@ -2481,12 +2491,12 @@
       <c r="R27" s="14"/>
       <c r="S27" s="5"/>
     </row>
-    <row r="28" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2497,7 +2507,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N28" s="11"/>
       <c r="O28" s="85"/>
@@ -2506,36 +2516,36 @@
       <c r="R28" s="14"/>
       <c r="S28" s="5"/>
     </row>
-    <row r="29" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K29" s="1"/>
       <c r="N29" s="11"/>
@@ -2545,7 +2555,7 @@
       <c r="R29" s="14"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
       <c r="O30" s="85"/>
@@ -2554,7 +2564,7 @@
       <c r="R30" s="14"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
       <c r="O31" s="85"/>
@@ -2563,7 +2573,7 @@
       <c r="R31" s="14"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
       <c r="O32" s="85"/>
@@ -2572,25 +2582,20 @@
       <c r="R32" s="14"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="G33" t="s">
-        <v>3</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
       <c r="O33" s="85"/>
@@ -2599,25 +2604,20 @@
       <c r="R33" s="14"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="G34" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
       <c r="M34" s="11"/>
       <c r="N34" s="11"/>
       <c r="O34" s="85"/>
@@ -2626,37 +2626,30 @@
       <c r="R34" s="14"/>
       <c r="S34" s="4"/>
     </row>
-    <row r="35" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
       <c r="O35" s="85"/>
@@ -2665,7 +2658,7 @@
       <c r="R35" s="14"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2673,27 +2666,22 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>80</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
       <c r="O36" s="85"/>
@@ -2702,7 +2690,7 @@
       <c r="R36" s="14"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -2714,17 +2702,10 @@
         <v>17</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="G37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
       <c r="M37" s="11"/>
       <c r="N37" s="11"/>
       <c r="O37" s="85"/>
@@ -2733,27 +2714,22 @@
       <c r="R37" s="14"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="G38" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
       <c r="M38" s="11"/>
       <c r="N38" s="11"/>
       <c r="O38" s="85"/>
@@ -2762,7 +2738,7 @@
       <c r="R38" s="14"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="M39" s="11"/>
@@ -2773,7 +2749,7 @@
       <c r="R39" s="14"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="M40" s="11"/>
@@ -2784,15 +2760,15 @@
       <c r="R40" s="14"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O41" s="88"/>
       <c r="P41" s="89"/>
       <c r="Q41" s="90"/>
       <c r="R41" s="16"/>
       <c r="S41" s="17"/>
     </row>
-    <row r="43" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B44" s="31" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +2783,7 @@
       <c r="K44" s="32"/>
       <c r="L44" s="33"/>
     </row>
-    <row r="45" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="34"/>
       <c r="C45" s="35"/>
       <c r="D45" s="35"/>
@@ -2820,7 +2796,7 @@
       <c r="K45" s="35"/>
       <c r="L45" s="36"/>
     </row>
-    <row r="46" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="37" t="s">
         <v>20</v>
       </c>
@@ -2837,10 +2813,10 @@
       <c r="K46" s="39"/>
       <c r="L46" s="40"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="38"/>
       <c r="C47" s="41" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D47" s="42"/>
       <c r="E47" s="42"/>
@@ -2852,7 +2828,7 @@
       <c r="K47" s="42"/>
       <c r="L47" s="43"/>
     </row>
-    <row r="48" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="38"/>
       <c r="C48" s="44" t="s">
         <v>22</v>
@@ -2867,7 +2843,7 @@
       <c r="K48" s="45"/>
       <c r="L48" s="46"/>
     </row>
-    <row r="49" spans="2:12" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:12" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B49" s="19" t="s">
         <v>23</v>
       </c>
@@ -2884,7 +2860,7 @@
       <c r="K49" s="23"/>
       <c r="L49" s="24"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="20"/>
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
@@ -2897,7 +2873,7 @@
       <c r="K50" s="25"/>
       <c r="L50" s="26"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="20"/>
       <c r="C51" s="27" t="s">
         <v>25</v>
@@ -2912,7 +2888,7 @@
       <c r="K51" s="27"/>
       <c r="L51" s="28"/>
     </row>
-    <row r="52" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="21"/>
       <c r="C52" s="29" t="s">
         <v>26</v>
@@ -2991,13 +2967,13 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -3008,9 +2984,9 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="2:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B5" s="120" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
@@ -3019,7 +2995,7 @@
       <c r="G5" s="120"/>
       <c r="H5" s="120"/>
       <c r="L5" s="121" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="M5" s="121"/>
       <c r="N5" s="121"/>
@@ -3028,9 +3004,9 @@
       <c r="Q5" s="121"/>
       <c r="R5" s="121"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="93" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C7" s="94"/>
       <c r="D7" s="94"/>
@@ -3039,7 +3015,7 @@
       <c r="G7" s="94"/>
       <c r="H7" s="95"/>
       <c r="L7" s="93" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="M7" s="94"/>
       <c r="N7" s="94"/>
@@ -3048,7 +3024,7 @@
       <c r="Q7" s="94"/>
       <c r="R7" s="95"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="96"/>
       <c r="C8" s="97"/>
       <c r="D8" s="97"/>
@@ -3064,9 +3040,9 @@
       <c r="Q8" s="97"/>
       <c r="R8" s="98"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="99" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C9" s="100"/>
       <c r="D9" s="100"/>
@@ -3075,7 +3051,7 @@
       <c r="G9" s="100"/>
       <c r="H9" s="101"/>
       <c r="L9" s="99" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="M9" s="100"/>
       <c r="N9" s="100"/>
@@ -3084,9 +3060,9 @@
       <c r="Q9" s="100"/>
       <c r="R9" s="101"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="91" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C10" s="86"/>
       <c r="D10" s="86"/>
@@ -3095,7 +3071,7 @@
       <c r="G10" s="86"/>
       <c r="H10" s="87"/>
       <c r="L10" s="91" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="M10" s="86"/>
       <c r="N10" s="86"/>
@@ -3104,9 +3080,9 @@
       <c r="Q10" s="86"/>
       <c r="R10" s="87"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="91" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C11" s="86"/>
       <c r="D11" s="86"/>
@@ -3115,7 +3091,7 @@
       <c r="G11" s="86"/>
       <c r="H11" s="87"/>
       <c r="L11" s="91" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="M11" s="86"/>
       <c r="N11" s="86"/>
@@ -3124,9 +3100,9 @@
       <c r="Q11" s="86"/>
       <c r="R11" s="87"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="91" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C12" s="86"/>
       <c r="D12" s="86"/>
@@ -3135,7 +3111,7 @@
       <c r="G12" s="86"/>
       <c r="H12" s="87"/>
       <c r="L12" s="91" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="M12" s="86"/>
       <c r="N12" s="86"/>
@@ -3144,9 +3120,9 @@
       <c r="Q12" s="86"/>
       <c r="R12" s="87"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="92" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
@@ -3162,9 +3138,9 @@
       <c r="Q13" s="48"/>
       <c r="R13" s="49"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="91" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
@@ -3173,7 +3149,7 @@
       <c r="G14" s="86"/>
       <c r="H14" s="87"/>
       <c r="L14" s="91" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="M14" s="86"/>
       <c r="N14" s="86"/>
@@ -3182,9 +3158,9 @@
       <c r="Q14" s="86"/>
       <c r="R14" s="87"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="91" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C15" s="86"/>
       <c r="D15" s="86"/>
@@ -3200,9 +3176,9 @@
       <c r="Q15" s="86"/>
       <c r="R15" s="87"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="105" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="106"/>
@@ -3211,7 +3187,7 @@
       <c r="G16" s="106"/>
       <c r="H16" s="107"/>
       <c r="L16" s="105" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M16" s="106"/>
       <c r="N16" s="106"/>
@@ -3220,9 +3196,9 @@
       <c r="Q16" s="106"/>
       <c r="R16" s="107"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="108" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C17" s="109"/>
       <c r="D17" s="109"/>
@@ -3231,7 +3207,7 @@
       <c r="G17" s="109"/>
       <c r="H17" s="110"/>
       <c r="L17" s="108" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="M17" s="109"/>
       <c r="N17" s="109"/>
@@ -3240,7 +3216,7 @@
       <c r="Q17" s="109"/>
       <c r="R17" s="110"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="111"/>
       <c r="C18" s="112"/>
       <c r="D18" s="112"/>
@@ -3256,9 +3232,9 @@
       <c r="Q18" s="112"/>
       <c r="R18" s="113"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="114" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C19" s="115"/>
       <c r="D19" s="115"/>
@@ -3267,7 +3243,7 @@
       <c r="G19" s="115"/>
       <c r="H19" s="116"/>
       <c r="L19" s="114" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="M19" s="115"/>
       <c r="N19" s="115"/>
@@ -3276,9 +3252,9 @@
       <c r="Q19" s="115"/>
       <c r="R19" s="116"/>
     </row>
-    <row r="20" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="102" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C20" s="103"/>
       <c r="D20" s="103"/>
@@ -3287,7 +3263,7 @@
       <c r="G20" s="103"/>
       <c r="H20" s="104"/>
       <c r="L20" s="122" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="M20" s="123"/>
       <c r="N20" s="123"/>
@@ -3296,7 +3272,7 @@
       <c r="Q20" s="123"/>
       <c r="R20" s="124"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="102"/>
       <c r="C21" s="103"/>
       <c r="D21" s="103"/>
@@ -3312,9 +3288,9 @@
       <c r="Q21" s="123"/>
       <c r="R21" s="124"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="102" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C22" s="103"/>
       <c r="D22" s="103"/>
@@ -3330,9 +3306,9 @@
       <c r="Q22" s="123"/>
       <c r="R22" s="124"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="102" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C23" s="103"/>
       <c r="D23" s="103"/>
@@ -3348,7 +3324,7 @@
       <c r="Q23" s="123"/>
       <c r="R23" s="124"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="102"/>
       <c r="C24" s="103"/>
       <c r="D24" s="103"/>
@@ -3364,7 +3340,7 @@
       <c r="Q24" s="123"/>
       <c r="R24" s="124"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="102"/>
       <c r="C25" s="103"/>
       <c r="D25" s="103"/>
@@ -3380,7 +3356,7 @@
       <c r="Q25" s="123"/>
       <c r="R25" s="124"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="102"/>
       <c r="C26" s="103"/>
       <c r="D26" s="103"/>
@@ -3396,7 +3372,7 @@
       <c r="Q26" s="123"/>
       <c r="R26" s="124"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="102"/>
       <c r="C27" s="103"/>
       <c r="D27" s="103"/>
@@ -3412,7 +3388,7 @@
       <c r="Q27" s="123"/>
       <c r="R27" s="124"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="102"/>
       <c r="C28" s="103"/>
       <c r="D28" s="103"/>
@@ -3428,7 +3404,7 @@
       <c r="Q28" s="123"/>
       <c r="R28" s="124"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="102"/>
       <c r="C29" s="103"/>
       <c r="D29" s="103"/>
@@ -3444,7 +3420,7 @@
       <c r="Q29" s="103"/>
       <c r="R29" s="104"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="102"/>
       <c r="C30" s="103"/>
       <c r="D30" s="103"/>
@@ -3460,7 +3436,7 @@
       <c r="Q30" s="103"/>
       <c r="R30" s="104"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="102"/>
       <c r="C31" s="103"/>
       <c r="D31" s="103"/>
@@ -3469,7 +3445,7 @@
       <c r="G31" s="103"/>
       <c r="H31" s="104"/>
       <c r="L31" s="102" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="M31" s="103"/>
       <c r="N31" s="103"/>
@@ -3478,7 +3454,7 @@
       <c r="Q31" s="103"/>
       <c r="R31" s="104"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="102"/>
       <c r="C32" s="103"/>
       <c r="D32" s="103"/>
@@ -3487,7 +3463,7 @@
       <c r="G32" s="103"/>
       <c r="H32" s="104"/>
       <c r="L32" s="102" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="M32" s="103"/>
       <c r="N32" s="103"/>
@@ -3496,7 +3472,7 @@
       <c r="Q32" s="103"/>
       <c r="R32" s="104"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="102"/>
       <c r="C33" s="103"/>
       <c r="D33" s="103"/>
@@ -3512,7 +3488,7 @@
       <c r="Q33" s="103"/>
       <c r="R33" s="104"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" s="102"/>
       <c r="C34" s="103"/>
       <c r="D34" s="103"/>
@@ -3528,7 +3504,7 @@
       <c r="Q34" s="103"/>
       <c r="R34" s="104"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B35" s="117"/>
       <c r="C35" s="118"/>
       <c r="D35" s="118"/>
@@ -3595,6 +3571,7 @@
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="B10:H10"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>